<commit_message>
AutoCommit_9 июля 2024 г. 21:52:09_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_УП.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_УП.xlsx
@@ -571,7 +571,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N2" sqref="N2"/>
+      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1026,6 +1026,9 @@
         <v>18</v>
       </c>
       <c r="D21" s="3"/>
+      <c r="J21">
+        <v>5</v>
+      </c>
       <c r="P21" s="3"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
@@ -1069,6 +1072,9 @@
       <c r="D23" s="2"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
+      <c r="J23">
+        <v>5</v>
+      </c>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="2"/>
@@ -1127,6 +1133,9 @@
       </c>
       <c r="D26" s="3"/>
       <c r="H26" s="4"/>
+      <c r="J26">
+        <v>5</v>
+      </c>
       <c r="P26" s="3"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
@@ -1147,6 +1156,9 @@
       </c>
       <c r="D27" s="3"/>
       <c r="H27" s="4"/>
+      <c r="J27">
+        <v>5</v>
+      </c>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 21:55:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_УП.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_УП.xlsx
@@ -571,7 +571,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J20" sqref="J20"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -847,7 +847,9 @@
       </c>
       <c r="D12" s="3"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="6">
+        <v>5</v>
+      </c>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="2"/>
@@ -1007,6 +1009,9 @@
         <v>17</v>
       </c>
       <c r="D20" s="3"/>
+      <c r="G20">
+        <v>5</v>
+      </c>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
@@ -1026,6 +1031,15 @@
         <v>18</v>
       </c>
       <c r="D21" s="3"/>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
       <c r="J21">
         <v>5</v>
       </c>
@@ -1070,8 +1084,15 @@
         <v>20</v>
       </c>
       <c r="D23" s="2"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="G23" s="4">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>5</v>
+      </c>
       <c r="J23">
         <v>5</v>
       </c>
@@ -1132,7 +1153,15 @@
         <v>23</v>
       </c>
       <c r="D26" s="3"/>
-      <c r="H26" s="4"/>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="H26" s="4">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>5</v>
+      </c>
       <c r="J26">
         <v>5</v>
       </c>
@@ -1155,7 +1184,15 @@
         <v>24</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="H27" s="4"/>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27" s="4">
+        <v>5</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
       <c r="J27">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 21:57:17_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_УП.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_УП.xlsx
@@ -571,7 +571,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,12 @@
       <c r="C20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3">
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
       <c r="G20">
         <v>5</v>
       </c>
@@ -1084,6 +1089,9 @@
         <v>20</v>
       </c>
       <c r="D23" s="2"/>
+      <c r="F23">
+        <v>5</v>
+      </c>
       <c r="G23" s="4">
         <v>5</v>
       </c>
@@ -1153,6 +1161,9 @@
         <v>23</v>
       </c>
       <c r="D26" s="3"/>
+      <c r="F26">
+        <v>5</v>
+      </c>
       <c r="G26">
         <v>5</v>
       </c>
@@ -1184,6 +1195,9 @@
         <v>24</v>
       </c>
       <c r="D27" s="3"/>
+      <c r="F27">
+        <v>5</v>
+      </c>
       <c r="G27">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 23:32:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_УП.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_УП.xlsx
@@ -571,7 +571,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -845,8 +845,12 @@
       <c r="C12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="F12" s="4"/>
+      <c r="D12" s="3">
+        <v>5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
       <c r="G12" s="6">
         <v>5</v>
       </c>
@@ -907,6 +911,9 @@
         <v>12</v>
       </c>
       <c r="D15" s="2"/>
+      <c r="G15">
+        <v>5</v>
+      </c>
       <c r="P15" s="3"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -1035,7 +1042,15 @@
       <c r="C21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
       <c r="G21">
         <v>5</v>
       </c>
@@ -1088,7 +1103,9 @@
       <c r="C23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2">
+        <v>5</v>
+      </c>
       <c r="F23">
         <v>5</v>
       </c>
@@ -1161,6 +1178,9 @@
         <v>23</v>
       </c>
       <c r="D26" s="3"/>
+      <c r="E26">
+        <v>5</v>
+      </c>
       <c r="F26">
         <v>5</v>
       </c>
@@ -1194,7 +1214,12 @@
       <c r="C27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3">
+        <v>5</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
       <c r="F27">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 23:51:56_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_УП.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_УП.xlsx
@@ -571,7 +571,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -684,6 +684,12 @@
       <c r="D4" s="5"/>
       <c r="G4" s="6"/>
       <c r="H4" s="4"/>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -768,6 +774,12 @@
       <c r="D8" s="3"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>5</v>
+      </c>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="2"/>
@@ -808,6 +820,12 @@
       <c r="D10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>5</v>
+      </c>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="2"/>
@@ -936,6 +954,12 @@
       <c r="E16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="4"/>
+      <c r="I16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <v>5</v>
+      </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
@@ -996,6 +1020,12 @@
       </c>
       <c r="D19" s="3"/>
       <c r="G19" s="4"/>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>5</v>
+      </c>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
       <c r="R19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_9 июля 2024 г. 23:52:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ОИБАС1022/2ОИБАС1022_УП.xlsx
+++ b/2ОИБАС1022/2ОИБАС1022_УП.xlsx
@@ -571,7 +571,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -820,6 +820,9 @@
       <c r="D10" s="3"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
+      <c r="H10">
+        <v>5</v>
+      </c>
       <c r="I10">
         <v>5</v>
       </c>
@@ -953,7 +956,9 @@
       <c r="D16" s="3"/>
       <c r="E16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
       <c r="I16">
         <v>5</v>
       </c>
@@ -1020,6 +1025,9 @@
       </c>
       <c r="D19" s="3"/>
       <c r="G19" s="4"/>
+      <c r="H19">
+        <v>5</v>
+      </c>
       <c r="I19">
         <v>5</v>
       </c>

</xml_diff>